<commit_message>
fix dkp and sell issue
</commit_message>
<xml_diff>
--- a/2019_dkp/current_dkp.xlsx
+++ b/2019_dkp/current_dkp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Blizzard\World of Warcraft\wow_dkp\2019_dkp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381FDEAB-15DE-47DC-AFA5-E8F5270CE770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC63302-E1C2-476F-BA35-8B125A993586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,203 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
-  <si>
-    <t>白色奶牛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>诶某某</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>哥顿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>光头强</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔道师傅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>鸽哨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>彼时年少</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>埃尔史密斯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>风雨者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>牛夫人如花</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黄小喵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>酥心果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡富贵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>施主来个馒头</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>寻找杰克船长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>凤凰山排骨男</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑矮星</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三季稻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>溺水的鱼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑暗小猫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>丁小沫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>好迟的糯米饭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>索道第一奶妈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>叨逼叨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>琺瑟厄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>岁月无恙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>那夜你好坏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Richard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>闻人微笑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我有虎牙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欺夜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑暗小猪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>传奇害一生</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡德财</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>天黑动手</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阿里之拳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>边个系一碌蔗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>丁小牛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>马果果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超级牛肉饭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>MC分数</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -241,10 +45,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>烟灰圈圈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>合计总分</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,14 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>血战半边天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>上次队伍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -279,6 +71,168 @@
   <si>
     <t>累积分数</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZS</t>
+  </si>
+  <si>
+    <t>白色奶牛</t>
+  </si>
+  <si>
+    <t>烟灰圈圈</t>
+  </si>
+  <si>
+    <t>诶某某</t>
+  </si>
+  <si>
+    <t>哥顿</t>
+  </si>
+  <si>
+    <t>Moy</t>
+  </si>
+  <si>
+    <t>光头强</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>魔道师傅</t>
+  </si>
+  <si>
+    <t>鸽哨</t>
+  </si>
+  <si>
+    <t>彼时年少</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>埃尔史密斯</t>
+  </si>
+  <si>
+    <t>风雨者</t>
+  </si>
+  <si>
+    <t>牛夫人如花</t>
+  </si>
+  <si>
+    <t>黄小喵</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>酥心果</t>
+  </si>
+  <si>
+    <t>亡富贵</t>
+  </si>
+  <si>
+    <t>施主来个馒头</t>
+  </si>
+  <si>
+    <t>寻找杰克船长</t>
+  </si>
+  <si>
+    <t>凤凰山排骨男</t>
+  </si>
+  <si>
+    <t>黑矮星</t>
+  </si>
+  <si>
+    <t>三季稻</t>
+  </si>
+  <si>
+    <t>溺水的鱼</t>
+  </si>
+  <si>
+    <t>黑暗小猫</t>
+  </si>
+  <si>
+    <t>血战半边天</t>
+  </si>
+  <si>
+    <t>丁沫沫</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>丁小沫</t>
+  </si>
+  <si>
+    <t>好迟的糯米饭</t>
+  </si>
+  <si>
+    <t>索道第一奶妈</t>
+  </si>
+  <si>
+    <t>叨逼叨</t>
+  </si>
+  <si>
+    <t>琺瑟厄</t>
+  </si>
+  <si>
+    <t>岁月无恙</t>
+  </si>
+  <si>
+    <t>那夜你好坏</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>闻人微笑</t>
+  </si>
+  <si>
+    <t>我有虎牙</t>
+  </si>
+  <si>
+    <t>欺夜</t>
+  </si>
+  <si>
+    <t>黑暗小猪</t>
+  </si>
+  <si>
+    <t>DZ</t>
+  </si>
+  <si>
+    <t>传奇害一生</t>
+  </si>
+  <si>
+    <t>亡德财</t>
+  </si>
+  <si>
+    <t>天黑动手</t>
+  </si>
+  <si>
+    <t>阿里之拳</t>
+  </si>
+  <si>
+    <t>边个系一碌蔗</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>丁小牛</t>
+  </si>
+  <si>
+    <t>马果果</t>
+  </si>
+  <si>
+    <t>超级牛肉饭</t>
+  </si>
+  <si>
+    <t>老牛太妖</t>
+  </si>
+  <si>
+    <t>jin</t>
   </si>
 </sst>
 </file>
@@ -656,13 +610,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P53"/>
+  <dimension ref="B2:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -678,13 +632,13 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G2" s="1" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
         <v>2</v>
@@ -692,42 +646,42 @@
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
@@ -747,18 +701,18 @@
       <c r="N4" s="8"/>
       <c r="O4" s="5"/>
       <c r="P4" s="9">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D5" s="5">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
@@ -778,18 +732,18 @@
       <c r="N5" s="8"/>
       <c r="O5" s="5"/>
       <c r="P5" s="9">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
@@ -809,18 +763,18 @@
       <c r="N6" s="8"/>
       <c r="O6" s="5"/>
       <c r="P6" s="9">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
@@ -840,18 +794,18 @@
       <c r="N7" s="8"/>
       <c r="O7" s="5"/>
       <c r="P7" s="9">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
@@ -871,15 +825,15 @@
       <c r="N8" s="8"/>
       <c r="O8" s="5"/>
       <c r="P8" s="9">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D9" s="5">
         <v>8</v>
@@ -930,13 +884,13 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D11" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
@@ -956,15 +910,15 @@
       <c r="N11" s="8"/>
       <c r="O11" s="5"/>
       <c r="P11" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
@@ -992,13 +946,13 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
@@ -1018,7 +972,7 @@
       <c r="N13" s="8"/>
       <c r="O13" s="5"/>
       <c r="P13" s="9">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
@@ -1046,13 +1000,13 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D15" s="5">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
@@ -1072,18 +1026,18 @@
       <c r="N15" s="8"/>
       <c r="O15" s="5"/>
       <c r="P15" s="9">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
@@ -1103,18 +1057,18 @@
       <c r="N16" s="8"/>
       <c r="O16" s="5"/>
       <c r="P16" s="9">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D17" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
@@ -1134,18 +1088,18 @@
       <c r="N17" s="8"/>
       <c r="O17" s="5"/>
       <c r="P17" s="9">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6"/>
@@ -1165,7 +1119,7 @@
       <c r="N18" s="8"/>
       <c r="O18" s="5"/>
       <c r="P18" s="9">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
@@ -1193,13 +1147,13 @@
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D20" s="5">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
@@ -1219,15 +1173,15 @@
       <c r="N20" s="8"/>
       <c r="O20" s="5"/>
       <c r="P20" s="9">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D21" s="5">
         <v>52</v>
@@ -1255,13 +1209,13 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D22" s="5">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
@@ -1281,15 +1235,15 @@
       <c r="N22" s="8"/>
       <c r="O22" s="5"/>
       <c r="P22" s="9">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
@@ -1317,13 +1271,13 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D24" s="5">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="6"/>
@@ -1343,18 +1297,18 @@
       <c r="N24" s="8"/>
       <c r="O24" s="5"/>
       <c r="P24" s="9">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D25" s="5">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="6"/>
@@ -1374,15 +1328,15 @@
       <c r="N25" s="8"/>
       <c r="O25" s="5"/>
       <c r="P25" s="9">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D26" s="5">
         <v>42</v>
@@ -1410,13 +1364,13 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D27" s="5">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -1436,18 +1390,18 @@
       <c r="N27" s="8"/>
       <c r="O27" s="5"/>
       <c r="P27" s="9">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D28" s="5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
@@ -1467,18 +1421,18 @@
       <c r="N28" s="8"/>
       <c r="O28" s="5"/>
       <c r="P28" s="9">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D29" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="6"/>
@@ -1498,13 +1452,19 @@
       <c r="N29" s="8"/>
       <c r="O29" s="5"/>
       <c r="P29" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
@@ -1522,18 +1482,14 @@
       </c>
       <c r="N30" s="8"/>
       <c r="O30" s="5"/>
-      <c r="P30" s="9"/>
+      <c r="P30" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="5">
-        <v>47</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="G31" s="7"/>
@@ -1551,19 +1507,17 @@
       </c>
       <c r="N31" s="8"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="9">
-        <v>47</v>
-      </c>
+      <c r="P31" s="9"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D32" s="5">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="6"/>
@@ -1583,18 +1537,18 @@
       <c r="N32" s="8"/>
       <c r="O32" s="5"/>
       <c r="P32" s="9">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D33" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="6"/>
@@ -1614,18 +1568,18 @@
       <c r="N33" s="8"/>
       <c r="O33" s="5"/>
       <c r="P33" s="9">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D34" s="5">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
@@ -1645,18 +1599,18 @@
       <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="9">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D35" s="5">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="6"/>
@@ -1676,18 +1630,18 @@
       <c r="N35" s="8"/>
       <c r="O35" s="5"/>
       <c r="P35" s="9">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D36" s="5">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="6"/>
@@ -1707,18 +1661,18 @@
       <c r="N36" s="8"/>
       <c r="O36" s="5"/>
       <c r="P36" s="9">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D37" s="5">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="6"/>
@@ -1738,18 +1692,18 @@
       <c r="N37" s="8"/>
       <c r="O37" s="5"/>
       <c r="P37" s="9">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D38" s="5">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="6"/>
@@ -1769,13 +1723,19 @@
       <c r="N38" s="8"/>
       <c r="O38" s="5"/>
       <c r="P38" s="9">
-        <v>12</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="5">
+        <v>18</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="6"/>
       <c r="G39" s="7"/>
@@ -1793,18 +1753,14 @@
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="5"/>
-      <c r="P39" s="9"/>
+      <c r="P39" s="9">
+        <v>18</v>
+      </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B40" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="5">
-        <v>43</v>
-      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="6"/>
       <c r="G40" s="7"/>
@@ -1822,19 +1778,17 @@
       </c>
       <c r="N40" s="8"/>
       <c r="O40" s="5"/>
-      <c r="P40" s="9">
-        <v>43</v>
-      </c>
+      <c r="P40" s="9"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D41" s="5">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="6"/>
@@ -1854,18 +1808,18 @@
       <c r="N41" s="8"/>
       <c r="O41" s="5"/>
       <c r="P41" s="9">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D42" s="5">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="6"/>
@@ -1885,18 +1839,18 @@
       <c r="N42" s="8"/>
       <c r="O42" s="5"/>
       <c r="P42" s="9">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D43" s="5">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="6"/>
@@ -1916,13 +1870,19 @@
       <c r="N43" s="8"/>
       <c r="O43" s="5"/>
       <c r="P43" s="9">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="5">
+        <v>30</v>
+      </c>
       <c r="E44" s="5"/>
       <c r="F44" s="6"/>
       <c r="G44" s="7"/>
@@ -1940,18 +1900,14 @@
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="5"/>
-      <c r="P44" s="9"/>
+      <c r="P44" s="9">
+        <v>30</v>
+      </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="5">
-        <v>14</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="6"/>
       <c r="G45" s="7"/>
@@ -1969,19 +1925,17 @@
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="5"/>
-      <c r="P45" s="9">
-        <v>14</v>
-      </c>
+      <c r="P45" s="9"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D46" s="5">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="6"/>
@@ -2001,18 +1955,18 @@
       <c r="N46" s="8"/>
       <c r="O46" s="5"/>
       <c r="P46" s="9">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D47" s="5">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="6"/>
@@ -2032,18 +1986,18 @@
       <c r="N47" s="8"/>
       <c r="O47" s="5"/>
       <c r="P47" s="9">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B48" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D48" s="5">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="6"/>
@@ -2063,18 +2017,18 @@
       <c r="N48" s="8"/>
       <c r="O48" s="5"/>
       <c r="P48" s="9">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D49" s="5">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="6"/>
@@ -2094,13 +2048,19 @@
       <c r="N49" s="8"/>
       <c r="O49" s="5"/>
       <c r="P49" s="9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="5">
+        <v>58</v>
+      </c>
       <c r="E50" s="5"/>
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
@@ -2118,14 +2078,16 @@
       </c>
       <c r="N50" s="8"/>
       <c r="O50" s="5"/>
-      <c r="P50" s="9"/>
+      <c r="P50" s="9">
+        <v>58</v>
+      </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="5" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D51" s="5">
         <v>6</v>
@@ -2152,15 +2114,9 @@
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" s="5">
-        <v>58</v>
-      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
@@ -2178,19 +2134,17 @@
       </c>
       <c r="N52" s="8"/>
       <c r="O52" s="5"/>
-      <c r="P52" s="9">
-        <v>58</v>
-      </c>
+      <c r="P52" s="9"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D53" s="5">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="6"/>
@@ -2210,7 +2164,107 @@
       <c r="N53" s="8"/>
       <c r="O53" s="5"/>
       <c r="P53" s="9">
-        <v>26</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="5">
+        <v>60</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="5">
+        <v>32</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56" s="5">
+        <v>6</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="5">
+        <v>4</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>